<commit_message>
funcao se exercicios de fixacao e revisao
</commit_message>
<xml_diff>
--- a/2.Excel/hands-on/6.Funcoes_Mercado/1.Funcao_SE.xlsx
+++ b/2.Excel/hands-on/6.Funcoes_Mercado/1.Funcao_SE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projetos para Github\Hashtag\2.Excel\hands-on\6.Funcoes_Mercado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79D4FFE-D88F-44F9-8C20-E832FC0C091E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95E584C-6F79-4850-BD7E-48BD2787DF6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="479" activeTab="1" xr2:uid="{85B08948-7BCF-4007-BABB-111144F4B1B5}"/>
+    <workbookView xWindow="12144" yWindow="0" windowWidth="10896" windowHeight="13056" tabRatio="479" activeTab="1" xr2:uid="{85B08948-7BCF-4007-BABB-111144F4B1B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Pratica1" sheetId="3" r:id="rId1"/>
@@ -2365,9 +2365,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2405,7 +2405,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2511,7 +2511,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2653,7 +2653,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2843,7 +2843,7 @@
   <dimension ref="A1:K4432"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4432"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>